<commit_message>
extended encoder navigation filter api + javadoc
</commit_message>
<xml_diff>
--- a/xml-coder/doc/Struktur.xlsx
+++ b/xml-coder/doc/Struktur.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="63">
   <si>
     <t>documentElement</t>
   </si>
@@ -180,7 +180,31 @@
     <t>0/1</t>
   </si>
   <si>
-    <t>yxdcxycyxc</t>
+    <t>navigationPathHash</t>
+  </si>
+  <si>
+    <t>navigationPathPool</t>
+  </si>
+  <si>
+    <t>Indices referenzierter Objekte.</t>
+  </si>
+  <si>
+    <t>Referenz in elementNamePool. Nur vorhanden, wenn uriPool leer ist.</t>
+  </si>
+  <si>
+    <t>Referenz in elementLabelPool. Nur vorhanden, wenn uriPool nicht leer ist.</t>
+  </si>
+  <si>
+    <t>Referenz in elementXmlnsPool. Nur vorhanden, wenn uriPool nicht leer ist.</t>
+  </si>
+  <si>
+    <t>Hash-Tabelle zum uriPool. Kann leer sein.</t>
+  </si>
+  <si>
+    <t>Referenz auf Document-Element im elementNodePool.</t>
+  </si>
+  <si>
+    <t>Anzahl der Elemente im Pool.</t>
   </si>
 </sst>
 </file>
@@ -230,7 +254,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -495,6 +519,19 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -502,7 +539,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -575,6 +612,50 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -584,50 +665,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Erklärender Text" xfId="1" builtinId="53"/>
@@ -930,30 +968,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H63"/>
+  <dimension ref="B2:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="26" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" style="42" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" style="39" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.28515625" style="51" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="67.140625" style="45" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="43"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
@@ -963,11 +1001,13 @@
       <c r="F3" s="12">
         <v>1</v>
       </c>
-      <c r="G3" s="29"/>
+      <c r="G3" s="29" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="4" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="35"/>
-      <c r="C4" s="44"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="48"/>
       <c r="D4" s="3" t="s">
         <v>23</v>
       </c>
@@ -977,14 +1017,12 @@
       <c r="F4" s="13">
         <v>1</v>
       </c>
-      <c r="G4" s="30" t="s">
-        <v>54</v>
-      </c>
+      <c r="G4" s="30"/>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="35"/>
-      <c r="C5" s="44"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="3" t="s">
         <v>27</v>
       </c>
@@ -998,8 +1036,8 @@
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" s="35"/>
-      <c r="C6" s="44"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="5" t="s">
         <v>26</v>
       </c>
@@ -1013,8 +1051,8 @@
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="35"/>
-      <c r="C7" s="44"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="5" t="s">
         <v>28</v>
       </c>
@@ -1028,8 +1066,8 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="35"/>
-      <c r="C8" s="44"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="48"/>
       <c r="D8" s="5" t="s">
         <v>29</v>
       </c>
@@ -1043,8 +1081,8 @@
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="35"/>
-      <c r="C9" s="44"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="48"/>
       <c r="D9" s="3" t="s">
         <v>30</v>
       </c>
@@ -1058,8 +1096,8 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
-      <c r="C10" s="44"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="48"/>
       <c r="D10" s="5" t="s">
         <v>31</v>
       </c>
@@ -1073,8 +1111,8 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="35"/>
-      <c r="C11" s="44"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="48"/>
       <c r="D11" s="3" t="s">
         <v>32</v>
       </c>
@@ -1088,8 +1126,8 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="35"/>
-      <c r="C12" s="44"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="5" t="s">
         <v>33</v>
       </c>
@@ -1103,8 +1141,8 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="35"/>
-      <c r="C13" s="44"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="48"/>
       <c r="D13" s="3" t="s">
         <v>35</v>
       </c>
@@ -1118,8 +1156,8 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="35"/>
-      <c r="C14" s="44"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="48"/>
       <c r="D14" s="5" t="s">
         <v>34</v>
       </c>
@@ -1133,8 +1171,8 @@
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="35"/>
-      <c r="C15" s="44"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="48"/>
       <c r="D15" s="5" t="s">
         <v>36</v>
       </c>
@@ -1148,8 +1186,8 @@
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B16" s="35"/>
-      <c r="C16" s="44"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="5" t="s">
         <v>37</v>
       </c>
@@ -1163,8 +1201,8 @@
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="35"/>
-      <c r="C17" s="44"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="48"/>
       <c r="D17" s="5" t="s">
         <v>38</v>
       </c>
@@ -1178,8 +1216,8 @@
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="35"/>
-      <c r="C18" s="44"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="48"/>
       <c r="D18" s="5" t="s">
         <v>39</v>
       </c>
@@ -1193,8 +1231,8 @@
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="35"/>
-      <c r="C19" s="44"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="48"/>
       <c r="D19" s="5" t="s">
         <v>40</v>
       </c>
@@ -1208,8 +1246,8 @@
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="35"/>
-      <c r="C20" s="44"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="48"/>
       <c r="D20" s="5" t="s">
         <v>41</v>
       </c>
@@ -1223,8 +1261,8 @@
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B21" s="35"/>
-      <c r="C21" s="44"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="48"/>
       <c r="D21" s="5" t="s">
         <v>42</v>
       </c>
@@ -1238,8 +1276,8 @@
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B22" s="35"/>
-      <c r="C22" s="44"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="48"/>
       <c r="D22" s="5" t="s">
         <v>43</v>
       </c>
@@ -1253,8 +1291,8 @@
       <c r="H22" s="4"/>
     </row>
     <row r="23" spans="2:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="B23" s="35"/>
-      <c r="C23" s="44"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="48"/>
       <c r="D23" s="5" t="s">
         <v>44</v>
       </c>
@@ -1267,449 +1305,491 @@
       <c r="G23" s="31"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="2:8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="36"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="8" t="s">
+    <row r="24" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B24" s="51"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="14">
+        <v>1</v>
+      </c>
+      <c r="G24" s="53"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="B25" s="51"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="14">
+        <v>1</v>
+      </c>
+      <c r="G25" s="53"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="2:8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="52"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E24" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="15">
-        <v>1</v>
-      </c>
-      <c r="G24" s="32"/>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="37" t="s">
+      <c r="E26" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="15">
+        <v>1</v>
+      </c>
+      <c r="G26" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="2" t="s">
+      <c r="C28" s="40"/>
+      <c r="D28" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="12">
-        <v>1</v>
-      </c>
-      <c r="G26" s="29"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="38"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="6" t="s">
+      <c r="E28" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="12">
+        <v>1</v>
+      </c>
+      <c r="G28" s="29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="35"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="16" t="s">
+      <c r="E29" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G27" s="31"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="38"/>
-      <c r="C28" s="47"/>
-      <c r="D28" s="6" t="s">
+      <c r="G29" s="31"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="35"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="16">
-        <v>1</v>
-      </c>
-      <c r="G28" s="31"/>
-    </row>
-    <row r="29" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="39"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="7" t="s">
+      <c r="E30" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="16">
+        <v>1</v>
+      </c>
+      <c r="G30" s="31"/>
+    </row>
+    <row r="31" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="36"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="F29" s="17" t="s">
+      <c r="E31" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="32"/>
-    </row>
-    <row r="30" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="46"/>
-      <c r="D31" s="2" t="s">
+      <c r="G31" s="32"/>
+    </row>
+    <row r="32" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="40"/>
+      <c r="D33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E33" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F33" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G31" s="29" t="s">
+      <c r="G33" s="29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="39"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="7" t="s">
+    <row r="34" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="36"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E32" s="26" t="s">
+      <c r="E34" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F34" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="32"/>
-    </row>
-    <row r="33" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="37" t="s">
+      <c r="G34" s="32"/>
+    </row>
+    <row r="35" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="46"/>
-      <c r="D34" s="2" t="s">
+      <c r="C36" s="40"/>
+      <c r="D36" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E34" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="12">
-        <v>1</v>
-      </c>
-      <c r="G34" s="29"/>
-    </row>
-    <row r="35" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="39"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="7" t="s">
+      <c r="E36" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="12">
+        <v>1</v>
+      </c>
+      <c r="G36" s="29"/>
+    </row>
+    <row r="37" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="36"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E35" s="26" t="s">
+      <c r="E37" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="17" t="s">
+      <c r="F37" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G35" s="32"/>
-    </row>
-    <row r="36" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="37" t="s">
+      <c r="G37" s="32"/>
+    </row>
+    <row r="38" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="D37" s="2" t="s">
+      <c r="C39" s="40"/>
+      <c r="D39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E37" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="12">
-        <v>1</v>
-      </c>
-      <c r="G37" s="29"/>
-    </row>
-    <row r="38" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="39"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="7" t="s">
+      <c r="E39" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="12">
+        <v>1</v>
+      </c>
+      <c r="G39" s="29"/>
+    </row>
+    <row r="40" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="36"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="17">
-        <v>1</v>
-      </c>
-      <c r="G38" s="32"/>
-    </row>
-    <row r="39" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="37" t="s">
+      <c r="E40" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="17">
+        <v>1</v>
+      </c>
+      <c r="G40" s="32"/>
+    </row>
+    <row r="41" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="46"/>
-      <c r="D40" s="2" t="s">
+      <c r="C42" s="40"/>
+      <c r="D42" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="12">
-        <v>1</v>
-      </c>
-      <c r="G40" s="29"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="38"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="6" t="s">
+      <c r="E42" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="12">
+        <v>1</v>
+      </c>
+      <c r="G42" s="29"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="35"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="16" t="s">
+      <c r="E43" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G41" s="31"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="38"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="6" t="s">
+      <c r="G43" s="31"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="35"/>
+      <c r="C44" s="41"/>
+      <c r="D44" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E42" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="16">
-        <v>1</v>
-      </c>
-      <c r="G42" s="31"/>
-    </row>
-    <row r="43" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="39"/>
-      <c r="C43" s="48"/>
-      <c r="D43" s="7" t="s">
+      <c r="E44" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="16">
+        <v>1</v>
+      </c>
+      <c r="G44" s="31"/>
+    </row>
+    <row r="45" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="36"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E43" s="26" t="s">
+      <c r="E45" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="F43" s="17" t="s">
+      <c r="F45" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G43" s="32"/>
-    </row>
-    <row r="44" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="37" t="s">
+      <c r="G45" s="32"/>
+    </row>
+    <row r="46" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C45" s="46"/>
-      <c r="D45" s="2" t="s">
+      <c r="C47" s="40"/>
+      <c r="D47" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E45" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" s="12" t="s">
+      <c r="E47" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G45" s="29"/>
-    </row>
-    <row r="46" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="39"/>
-      <c r="C46" s="48"/>
-      <c r="D46" s="7" t="s">
+      <c r="G47" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="36"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E46" s="26" t="s">
+      <c r="E48" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="17" t="s">
+      <c r="F48" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G46" s="32"/>
-    </row>
-    <row r="47" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="37" t="s">
+      <c r="G48" s="32"/>
+    </row>
+    <row r="49" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="46"/>
-      <c r="D48" s="2" t="s">
+      <c r="C50" s="40"/>
+      <c r="D50" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E48" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="12">
-        <v>1</v>
-      </c>
-      <c r="G48" s="29"/>
-    </row>
-    <row r="49" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="39"/>
-      <c r="C49" s="48"/>
-      <c r="D49" s="7" t="s">
+      <c r="E50" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="12">
+        <v>1</v>
+      </c>
+      <c r="G50" s="29"/>
+    </row>
+    <row r="51" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="36"/>
+      <c r="C51" s="42"/>
+      <c r="D51" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E49" s="26" t="s">
+      <c r="E51" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="F49" s="17" t="s">
+      <c r="F51" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G49" s="32"/>
-    </row>
-    <row r="51" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="37" t="s">
+      <c r="G51" s="32"/>
+    </row>
+    <row r="53" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C52" s="46"/>
-      <c r="D52" s="2" t="s">
+      <c r="C54" s="40"/>
+      <c r="D54" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E52" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="12" t="s">
+      <c r="E54" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G52" s="29"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="40"/>
-      <c r="C53" s="49"/>
-      <c r="D53" s="10" t="s">
+      <c r="G54" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="37"/>
+      <c r="C55" s="43"/>
+      <c r="D55" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E53" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="18" t="s">
+      <c r="E55" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="G53" s="30"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="38"/>
-      <c r="C54" s="47"/>
-      <c r="D54" s="6" t="s">
+      <c r="G55" s="30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="35"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E54" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54" s="16" t="s">
+      <c r="E56" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="G54" s="31"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="38"/>
-      <c r="C55" s="47"/>
-      <c r="D55" s="6" t="s">
+      <c r="G56" s="31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="35"/>
+      <c r="C57" s="41"/>
+      <c r="D57" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E55" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="19">
-        <v>1</v>
-      </c>
-      <c r="G55" s="31"/>
-    </row>
-    <row r="56" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="39"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="7" t="s">
+      <c r="E57" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" s="19">
+        <v>1</v>
+      </c>
+      <c r="G57" s="31"/>
+    </row>
+    <row r="58" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="36"/>
+      <c r="C58" s="42"/>
+      <c r="D58" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E56" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="17">
-        <v>1</v>
-      </c>
-      <c r="G56" s="32"/>
-    </row>
-    <row r="57" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="37" t="s">
+      <c r="E58" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="17">
+        <v>1</v>
+      </c>
+      <c r="G58" s="32"/>
+    </row>
+    <row r="59" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C58" s="46"/>
-      <c r="D58" s="2" t="s">
+      <c r="C60" s="40"/>
+      <c r="D60" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="12">
-        <v>1</v>
-      </c>
-      <c r="G58" s="29"/>
-    </row>
-    <row r="59" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="39"/>
-      <c r="C59" s="48"/>
-      <c r="D59" s="7" t="s">
+      <c r="E60" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="12">
+        <v>1</v>
+      </c>
+      <c r="G60" s="29"/>
+    </row>
+    <row r="61" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="36"/>
+      <c r="C61" s="42"/>
+      <c r="D61" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E59" s="26" t="s">
+      <c r="E61" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="F59" s="17" t="s">
+      <c r="F61" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G59" s="32"/>
-    </row>
-    <row r="60" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="37" t="s">
+      <c r="G61" s="32"/>
+    </row>
+    <row r="62" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C61" s="46"/>
-      <c r="D61" s="2" t="s">
+      <c r="C63" s="40"/>
+      <c r="D63" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E61" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61" s="12" t="s">
+      <c r="E63" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G61" s="29"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="41"/>
-      <c r="C62" s="50"/>
-      <c r="D62" s="9" t="s">
+      <c r="G63" s="29"/>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="38"/>
+      <c r="C64" s="44"/>
+      <c r="D64" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E62" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62" s="18" t="s">
+      <c r="E64" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="G62" s="52"/>
-    </row>
-    <row r="63" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="39"/>
-      <c r="C63" s="48"/>
-      <c r="D63" s="7" t="s">
+      <c r="G64" s="46"/>
+    </row>
+    <row r="65" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="36"/>
+      <c r="C65" s="42"/>
+      <c r="D65" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E63" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63" s="17">
-        <v>1</v>
-      </c>
-      <c r="G63" s="32"/>
+      <c r="E65" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="17">
+        <v>1</v>
+      </c>
+      <c r="G65" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C3:C24"/>
-    <mergeCell ref="B3:B24"/>
+    <mergeCell ref="C3:C26"/>
+    <mergeCell ref="B3:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>